<commit_message>
first version with user preference
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/check_protocol/sein ganglions.xlsx
+++ b/Plancheck/plancheck_data/check_protocol/sein ganglions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="163">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -511,10 +511,7 @@
     <t>RingPTVSein</t>
   </si>
   <si>
-    <t>PlexusGche</t>
-  </si>
-  <si>
-    <t>PlexusDt</t>
+    <t>Plexus Brachial</t>
   </si>
 </sst>
 </file>
@@ -1501,7 +1498,7 @@
   </sheetPr>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2306,10 +2303,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2469,13 +2466,10 @@
       <c r="A22" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="C22" s="12">
-        <v>1</v>
-      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
       <c r="C23" s="12">
         <v>1</v>
@@ -2483,7 +2477,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C24" s="12">
         <v>1</v>
@@ -2491,17 +2485,9 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C25" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" s="12">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
debug old tomo report
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/check_protocol/sein ganglions.xlsx
+++ b/Plancheck/plancheck_data/check_protocol/sein ganglions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -1498,7 +1498,7 @@
   </sheetPr>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1547,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
@@ -2305,7 +2305,7 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>

</xml_diff>